<commit_message>
data for new study extracted
</commit_message>
<xml_diff>
--- a/data/meta_table_filled.xlsx
+++ b/data/meta_table_filled.xlsx
@@ -9,17 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="30620" yWindow="460" windowWidth="36460" windowHeight="20140"/>
+    <workbookView xWindow="39180" yWindow="3100" windowWidth="28800" windowHeight="16520"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="explanations" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1832" uniqueCount="1272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1843" uniqueCount="1283">
   <si>
     <t>Key</t>
   </si>
@@ -3835,6 +3836,39 @@
   </si>
   <si>
     <t>Great tit</t>
+  </si>
+  <si>
+    <t>No sufficient repeatabilities reported / analysed</t>
+  </si>
+  <si>
+    <t>Data is there (Paper 3 in R script) Not yet analysed</t>
+  </si>
+  <si>
+    <t>To be figured out</t>
+  </si>
+  <si>
+    <t>To be analysed or with open questions (data is there in R script)</t>
+  </si>
+  <si>
+    <t>Meta Table constructed in R with data available</t>
+  </si>
+  <si>
+    <t>Meta Table constructed in R without info from paper</t>
+  </si>
+  <si>
+    <t>Only one repeatability reported / no data</t>
+  </si>
+  <si>
+    <t>No repeatability reported</t>
+  </si>
+  <si>
+    <t>Strange way of reporting, things are a bit unclear.</t>
+  </si>
+  <si>
+    <t>Only one repeatability reported / no data / only short term and 3 measurements</t>
+  </si>
+  <si>
+    <t>10 measurements but only one repeatability reported</t>
   </si>
 </sst>
 </file>
@@ -3858,7 +3892,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3901,6 +3935,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -3914,7 +3960,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3926,6 +3972,10 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4271,9 +4321,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB253"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AB7" sqref="AB7"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AB54" sqref="AB54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7053,58 +7103,58 @@
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+    <row r="42" spans="1:28" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="C42">
+      <c r="C42" s="10">
         <v>2015</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D42" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="E42" t="s">
+      <c r="E42" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="H42" t="s">
+      <c r="H42" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="I42" t="s">
+      <c r="I42" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="J42">
+      <c r="J42" s="10">
         <v>108</v>
       </c>
-      <c r="K42" s="3" t="s">
+      <c r="K42" s="10" t="s">
         <v>1271</v>
       </c>
     </row>
-    <row r="43" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+    <row r="43" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="C43">
+      <c r="C43" s="9">
         <v>2017</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D43" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="E43" t="s">
+      <c r="E43" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="H43" t="s">
+      <c r="H43" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="I43" t="s">
+      <c r="I43" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="J43">
+      <c r="J43" s="9">
         <v>86</v>
       </c>
     </row>
@@ -7137,29 +7187,29 @@
         <v>1268</v>
       </c>
     </row>
-    <row r="45" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
+    <row r="45" spans="1:28" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="C45">
+      <c r="C45" s="5">
         <v>2017</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D45" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="E45" t="s">
+      <c r="E45" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="H45" t="s">
+      <c r="H45" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="I45" t="s">
+      <c r="I45" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="J45">
+      <c r="J45" s="5">
         <v>20</v>
       </c>
     </row>
@@ -7192,215 +7242,230 @@
         <v>1269</v>
       </c>
     </row>
-    <row r="47" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
+    <row r="47" spans="1:28" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="C47">
+      <c r="C47" s="10">
         <v>2017</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D47" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="E47" t="s">
+      <c r="E47" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="H47" t="s">
+      <c r="H47" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="I47" t="s">
+      <c r="I47" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="J47">
+      <c r="J47" s="10">
         <v>189</v>
       </c>
     </row>
-    <row r="48" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
+    <row r="48" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C48">
+      <c r="C48" s="2">
         <v>2018</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D48" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="E48" t="s">
+      <c r="E48" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="H48" t="s">
+      <c r="H48" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="I48" t="s">
+      <c r="I48" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="J48">
+      <c r="J48" s="2">
         <v>136</v>
       </c>
-    </row>
-    <row r="49" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
+      <c r="AB48" s="2" t="s">
+        <v>1278</v>
+      </c>
+    </row>
+    <row r="49" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="C49">
+      <c r="C49" s="2">
         <v>2012</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D49" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="E49" t="s">
+      <c r="E49" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="G49" t="s">
+      <c r="G49" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="H49" t="s">
+      <c r="H49" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="I49" t="s">
+      <c r="I49" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="J49">
+      <c r="J49" s="2">
         <v>105</v>
       </c>
-    </row>
-    <row r="50" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
+      <c r="AB49" s="2" t="s">
+        <v>1279</v>
+      </c>
+    </row>
+    <row r="50" spans="1:28" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="C50">
+      <c r="C50" s="12">
         <v>2004</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D50" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="E50" t="s">
+      <c r="E50" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="H50" t="s">
+      <c r="H50" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="I50" t="s">
+      <c r="I50" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="J50">
+      <c r="J50" s="12">
         <v>57</v>
       </c>
     </row>
-    <row r="51" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
+    <row r="51" spans="1:28" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="C51">
+      <c r="C51" s="5">
         <v>2017</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D51" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="E51" t="s">
+      <c r="E51" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="G51" t="s">
+      <c r="G51" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="H51" t="s">
+      <c r="H51" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="J51">
+      <c r="J51" s="5">
         <v>8</v>
       </c>
-    </row>
-    <row r="52" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
+      <c r="AB51" s="5" t="s">
+        <v>1273</v>
+      </c>
+    </row>
+    <row r="52" spans="1:28" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="C52">
+      <c r="C52" s="12">
         <v>2013</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D52" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="E52" t="s">
+      <c r="E52" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="H52" t="s">
+      <c r="H52" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="I52" t="s">
+      <c r="I52" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="J52">
+      <c r="J52" s="12">
         <v>182</v>
       </c>
-    </row>
-    <row r="53" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
+      <c r="AB52" s="12" t="s">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="53" spans="1:28" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B53" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="C53">
+      <c r="C53" s="12">
         <v>2013</v>
       </c>
-      <c r="D53" t="s">
+      <c r="D53" s="12" t="s">
         <v>125</v>
       </c>
-      <c r="E53" t="s">
+      <c r="E53" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="H53" t="s">
+      <c r="H53" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="I53" t="s">
+      <c r="I53" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="J53">
+      <c r="J53" s="12">
         <v>150</v>
       </c>
     </row>
-    <row r="54" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
+    <row r="54" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B54" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="C54">
+      <c r="C54" s="6">
         <v>2016</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D54" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="E54" t="s">
+      <c r="E54" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="H54" t="s">
+      <c r="H54" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="I54" t="s">
+      <c r="I54" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="J54">
+      <c r="J54" s="6">
         <v>6</v>
+      </c>
+      <c r="AB54" s="6" t="s">
+        <v>1282</v>
       </c>
     </row>
     <row r="55" spans="1:28" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -7432,30 +7497,33 @@
         <v>1267</v>
       </c>
     </row>
-    <row r="56" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
+    <row r="56" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="C56">
+      <c r="C56" s="6">
         <v>2017</v>
       </c>
-      <c r="D56" t="s">
+      <c r="D56" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="E56" t="s">
+      <c r="E56" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="H56" t="s">
+      <c r="H56" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="I56" t="s">
+      <c r="I56" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="J56">
+      <c r="J56" s="6">
         <v>123</v>
+      </c>
+      <c r="AB56" s="2" t="s">
+        <v>1281</v>
       </c>
     </row>
     <row r="57" spans="1:28" x14ac:dyDescent="0.2">
@@ -12551,4 +12619,50 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C7:M11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="5" width="22.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="7" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C7" t="s">
+        <v>1276</v>
+      </c>
+      <c r="F7" t="s">
+        <v>1272</v>
+      </c>
+      <c r="J7" t="s">
+        <v>1275</v>
+      </c>
+      <c r="M7" t="s">
+        <v>1274</v>
+      </c>
+    </row>
+    <row r="8" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C8" s="7"/>
+      <c r="F8" s="6"/>
+      <c r="J8" s="5"/>
+      <c r="M8" s="9"/>
+    </row>
+    <row r="10" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C10" s="11" t="s">
+        <v>1277</v>
+      </c>
+    </row>
+    <row r="11" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C11" s="10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>